<commit_message>
Corrigindo e adicionando tempos.
</commit_message>
<xml_diff>
--- a/recursos/Tempo-PBL.xlsx
+++ b/recursos/Tempo-PBL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Optimus 2020\Desktop\Problema 1\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5873A10A-126F-4AFF-8F63-3EF9155E3C17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982A1965-AD1A-4EC4-895D-A6F3E7489201}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{9B8E14A5-E52C-4BCD-8500-9C3996E07EF0}"/>
   </bookViews>
@@ -91,7 +91,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +107,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,9 +146,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -157,6 +160,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,7 +481,7 @@
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,262 +493,266 @@
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>10</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="6">
         <v>50</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="6">
         <v>100</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="6">
         <v>500</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="6">
         <v>1000</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="6">
         <v>5000</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="6">
         <v>10000</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>4.6900000000000002E-4</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>3.712E-3</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0.58691300000000002</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>5.9876880000000003</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>1773.548237</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>27570.523415</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3">
-        <v>24358.291609</v>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2">
+        <v>24319.558530999999</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2">
+        <v>24339.005288</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="6">
         <v>10</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="6">
         <v>50</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="6">
         <v>100</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="6">
         <v>500</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="6">
         <v>1000</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="6">
         <v>5000</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="6">
         <v>10000</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>3.0000000000000001E-6</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>2.7599999999999999E-4</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>2.2300000000000002E-3</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>0.303844</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>2.9630320000000001</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>1392.233616</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>21340.955129999998</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3">
-        <v>21502.151020000001</v>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2">
+        <v>21471.753570000001</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3">
-        <v>15592.44752</v>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2">
+        <v>15552.265799999999</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2">
+        <v>22439.233189999999</v>
+      </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Adicionando 4 tempo multiplicação 10K em linguagem C.
</commit_message>
<xml_diff>
--- a/recursos/Tempo-PBL.xlsx
+++ b/recursos/Tempo-PBL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Optimus 2020\Desktop\Problema 1\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982A1965-AD1A-4EC4-895D-A6F3E7489201}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6539755-2FB4-4E7C-A4D3-9FFDFE5A7184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{9B8E14A5-E52C-4BCD-8500-9C3996E07EF0}"/>
   </bookViews>
@@ -155,14 +155,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,7 +481,7 @@
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,52 +497,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>10</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>50</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>100</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>500</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>1000</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>5000</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="4">
         <v>10000</v>
       </c>
     </row>
@@ -610,7 +610,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="I8" s="2">
+        <v>29160.816735</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
@@ -623,52 +625,52 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>10</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>50</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>100</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <v>500</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <v>1000</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <v>5000</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="4">
         <v>10000</v>
       </c>
     </row>
@@ -741,18 +743,18 @@
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Todos os tempos m5k linguagem C.
</commit_message>
<xml_diff>
--- a/recursos/Tempo-PBL.xlsx
+++ b/recursos/Tempo-PBL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Optimus 2020\Desktop\Problema 1\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6539755-2FB4-4E7C-A4D3-9FFDFE5A7184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC14B47-2078-4238-97E8-E8B4C865D7E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{9B8E14A5-E52C-4BCD-8500-9C3996E07EF0}"/>
   </bookViews>
@@ -76,7 +76,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +86,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,6 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8576F20F-689C-458D-97B1-4756071EF9E4}">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +590,9 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>1730.3349800000001</v>
+      </c>
       <c r="I6" s="2">
         <v>24319.558530999999</v>
       </c>
@@ -595,7 +606,9 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>1690.43894</v>
+      </c>
       <c r="I7" s="2">
         <v>24339.005288</v>
       </c>
@@ -609,7 +622,9 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>1677.2099900000001</v>
+      </c>
       <c r="I8" s="2">
         <v>29160.816735</v>
       </c>
@@ -742,19 +757,22 @@
         <v>22439.233189999999</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D18" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D19" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
+    </row>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Adicionando todos os tempos.
</commit_message>
<xml_diff>
--- a/recursos/Tempo-PBL.xlsx
+++ b/recursos/Tempo-PBL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Optimus 2020\Desktop\Problema 1\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC14B47-2078-4238-97E8-E8B4C865D7E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B641001-6BE2-4AAE-98FB-BFC205887A05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{9B8E14A5-E52C-4BCD-8500-9C3996E07EF0}"/>
   </bookViews>
@@ -166,13 +166,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,7 +490,7 @@
   <dimension ref="B2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,28 +506,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -585,11 +585,21 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="C6" s="2">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4.6900000000000002E-4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3.7200000000000002E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.59293799999999997</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5.6170660000000003</v>
+      </c>
       <c r="H6" s="2">
         <v>1730.3349800000001</v>
       </c>
@@ -601,11 +611,21 @@
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="C7" s="2">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.7199999999999998E-4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3.7100000000000002E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.57669400000000004</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5.7696490000000002</v>
+      </c>
       <c r="H7" s="2">
         <v>1690.43894</v>
       </c>
@@ -617,11 +637,21 @@
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="C8" s="2">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.7399999999999997E-4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3.7299999999999998E-3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.59188099999999999</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5.8936479999999998</v>
+      </c>
       <c r="H8" s="2">
         <v>1677.2099900000001</v>
       </c>
@@ -640,28 +670,28 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -719,12 +749,24 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="C14" s="2">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2.7500000000000002E-4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.2430000000000002E-3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.30212499999999998</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2.5435300000000001</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1386.16563</v>
+      </c>
       <c r="I14" s="2">
         <v>21471.753570000001</v>
       </c>
@@ -733,12 +775,24 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="C15" s="2">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2.7599999999999999E-4</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2.258E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.30479699999999998</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2.5441699999999998</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1359.10005</v>
+      </c>
       <c r="I15" s="2">
         <v>15552.265799999999</v>
       </c>
@@ -747,32 +801,44 @@
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="C16" s="2">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2.7099999999999997E-4</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2.2420000000000001E-3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.30190600000000001</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2.5185300000000002</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1389.1965499999999</v>
+      </c>
       <c r="I16" s="2">
         <v>22439.233189999999</v>
       </c>
     </row>
     <row r="18" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="21" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M21" s="7"/>
+      <c r="M21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>